<commit_message>
feat: Enhance job search functionality with localized labels and improved filtering options
</commit_message>
<xml_diff>
--- a/LIS_Diagnostics_moyen_terme_2024-2028_516_professions.xlsx
+++ b/LIS_Diagnostics_moyen_terme_2024-2028_516_professions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\pstq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C3231B-D141-4417-B2C0-F8B4DF91916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4C84B7-74B4-4C04-BF0A-97C5493DD937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15045" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15045" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagnostics_2024_2028" sheetId="4" r:id="rId1"/>
@@ -3666,16 +3666,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73F14DE-B5AF-457D-BD84-E38D1B6C52C5}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F517"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="43.88671875" customWidth="1"/>
     <col min="3" max="3" width="28.21875" customWidth="1"/>
     <col min="4" max="4" width="12.109375" customWidth="1"/>
@@ -3703,7 +3702,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -3743,7 +3742,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -3803,7 +3802,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10021</v>
       </c>
@@ -3943,7 +3942,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10022</v>
       </c>
@@ -3963,7 +3962,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10029</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10030</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11101</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>11103</v>
       </c>
@@ -4083,7 +4082,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>11109</v>
       </c>
@@ -4163,7 +4162,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12010</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12011</v>
       </c>
@@ -4203,7 +4202,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>12012</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>12013</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>12100</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>12103</v>
       </c>
@@ -4323,7 +4322,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>12104</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>12110</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>12112</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>12113</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>13102</v>
       </c>
@@ -4603,7 +4602,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>13112</v>
       </c>
@@ -4623,7 +4622,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>13200</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>14100</v>
       </c>
@@ -4683,7 +4682,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>14101</v>
       </c>
@@ -4703,7 +4702,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>14102</v>
       </c>
@@ -4723,7 +4722,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>14103</v>
       </c>
@@ -4743,7 +4742,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>14110</v>
       </c>
@@ -4763,7 +4762,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>14111</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>14112</v>
       </c>
@@ -4803,7 +4802,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14200</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>14201</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>14202</v>
       </c>
@@ -4863,7 +4862,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>14300</v>
       </c>
@@ -4883,7 +4882,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>14301</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>14400</v>
       </c>
@@ -4943,7 +4942,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14402</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20010</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20011</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20012</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>21100</v>
       </c>
@@ -5103,7 +5102,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>21101</v>
       </c>
@@ -5123,7 +5122,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>21102</v>
       </c>
@@ -5143,7 +5142,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>21103</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>21109</v>
       </c>
@@ -5183,7 +5182,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>21110</v>
       </c>
@@ -5203,7 +5202,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>21111</v>
       </c>
@@ -5223,7 +5222,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>21112</v>
       </c>
@@ -5243,7 +5242,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>21120</v>
       </c>
@@ -5263,7 +5262,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>21200</v>
       </c>
@@ -5283,7 +5282,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>21201</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21202</v>
       </c>
@@ -5323,7 +5322,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>21203</v>
       </c>
@@ -5343,7 +5342,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>21210</v>
       </c>
@@ -5363,7 +5362,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>21211</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>21220</v>
       </c>
@@ -5403,7 +5402,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>21221</v>
       </c>
@@ -5423,7 +5422,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>21222</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>21223</v>
       </c>
@@ -5463,7 +5462,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>21230</v>
       </c>
@@ -5483,7 +5482,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>21231</v>
       </c>
@@ -5503,7 +5502,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>21232</v>
       </c>
@@ -5523,7 +5522,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>21233</v>
       </c>
@@ -5543,7 +5542,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>21234</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>21300</v>
       </c>
@@ -5583,7 +5582,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>21301</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>21310</v>
       </c>
@@ -5623,7 +5622,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>21311</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>21320</v>
       </c>
@@ -5663,7 +5662,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>21321</v>
       </c>
@@ -5683,7 +5682,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>21322</v>
       </c>
@@ -5703,7 +5702,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>21330</v>
       </c>
@@ -5723,7 +5722,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>21331</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>21332</v>
       </c>
@@ -5763,7 +5762,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>21390</v>
       </c>
@@ -5783,7 +5782,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>21399</v>
       </c>
@@ -5803,7 +5802,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>22100</v>
       </c>
@@ -5823,7 +5822,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>22101</v>
       </c>
@@ -5843,7 +5842,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>22110</v>
       </c>
@@ -5863,7 +5862,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>22111</v>
       </c>
@@ -5883,7 +5882,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>22112</v>
       </c>
@@ -5903,7 +5902,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>22113</v>
       </c>
@@ -5923,7 +5922,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>22114</v>
       </c>
@@ -5943,7 +5942,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>22210</v>
       </c>
@@ -5963,7 +5962,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>22211</v>
       </c>
@@ -5983,7 +5982,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>22212</v>
       </c>
@@ -6003,7 +6002,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>22213</v>
       </c>
@@ -6023,7 +6022,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>22214</v>
       </c>
@@ -6043,7 +6042,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>22220</v>
       </c>
@@ -6063,7 +6062,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>22221</v>
       </c>
@@ -6083,7 +6082,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>22222</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>22230</v>
       </c>
@@ -6123,7 +6122,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>22231</v>
       </c>
@@ -6143,7 +6142,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>22232</v>
       </c>
@@ -6163,7 +6162,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>22233</v>
       </c>
@@ -6183,7 +6182,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>22300</v>
       </c>
@@ -6203,7 +6202,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>22301</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>22302</v>
       </c>
@@ -6243,7 +6242,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>22303</v>
       </c>
@@ -6263,7 +6262,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>22310</v>
       </c>
@@ -6283,7 +6282,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>22311</v>
       </c>
@@ -6303,7 +6302,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>22312</v>
       </c>
@@ -6323,7 +6322,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>22313</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>30010</v>
       </c>
@@ -6363,7 +6362,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>31100</v>
       </c>
@@ -6383,7 +6382,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>31101</v>
       </c>
@@ -6403,7 +6402,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>31102</v>
       </c>
@@ -6423,7 +6422,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>31103</v>
       </c>
@@ -6443,7 +6442,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>31110</v>
       </c>
@@ -6463,7 +6462,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>31111</v>
       </c>
@@ -6483,7 +6482,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>31112</v>
       </c>
@@ -6503,7 +6502,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>31120</v>
       </c>
@@ -6523,7 +6522,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>31121</v>
       </c>
@@ -6543,7 +6542,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>31200</v>
       </c>
@@ -6563,7 +6562,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>31201</v>
       </c>
@@ -6583,7 +6582,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>31202</v>
       </c>
@@ -6603,7 +6602,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>31203</v>
       </c>
@@ -6623,7 +6622,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>31204</v>
       </c>
@@ -6643,7 +6642,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>31209</v>
       </c>
@@ -6663,7 +6662,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>31300</v>
       </c>
@@ -6683,7 +6682,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>31301</v>
       </c>
@@ -6703,7 +6702,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>31302</v>
       </c>
@@ -6723,7 +6722,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>31303</v>
       </c>
@@ -6743,7 +6742,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>32100</v>
       </c>
@@ -6763,7 +6762,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>32101</v>
       </c>
@@ -6783,7 +6782,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>32102</v>
       </c>
@@ -6803,7 +6802,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>32103</v>
       </c>
@@ -6823,7 +6822,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>32104</v>
       </c>
@@ -6843,7 +6842,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>32109</v>
       </c>
@@ -6863,7 +6862,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>32110</v>
       </c>
@@ -6883,7 +6882,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>32111</v>
       </c>
@@ -6903,7 +6902,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>32112</v>
       </c>
@@ -6923,7 +6922,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>32120</v>
       </c>
@@ -6943,7 +6942,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>32121</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>32122</v>
       </c>
@@ -6983,7 +6982,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>32123</v>
       </c>
@@ -7003,7 +7002,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>32124</v>
       </c>
@@ -7023,7 +7022,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>32129</v>
       </c>
@@ -7043,7 +7042,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>32200</v>
       </c>
@@ -7063,7 +7062,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>32201</v>
       </c>
@@ -7083,7 +7082,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>32209</v>
       </c>
@@ -7103,7 +7102,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>33100</v>
       </c>
@@ -7123,7 +7122,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>33101</v>
       </c>
@@ -7143,7 +7142,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>33102</v>
       </c>
@@ -7163,7 +7162,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>33103</v>
       </c>
@@ -7183,7 +7182,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>33109</v>
       </c>
@@ -7203,7 +7202,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>40010</v>
       </c>
@@ -7223,7 +7222,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>40011</v>
       </c>
@@ -7243,7 +7242,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>40012</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>40019</v>
       </c>
@@ -7283,7 +7282,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>40020</v>
       </c>
@@ -7303,7 +7302,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>40021</v>
       </c>
@@ -7323,7 +7322,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>40030</v>
       </c>
@@ -7343,7 +7342,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>40040</v>
       </c>
@@ -7363,7 +7362,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>40041</v>
       </c>
@@ -7383,7 +7382,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>40042</v>
       </c>
@@ -7403,7 +7402,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>41100</v>
       </c>
@@ -7423,7 +7422,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>41101</v>
       </c>
@@ -7443,7 +7442,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>41200</v>
       </c>
@@ -7463,7 +7462,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>41201</v>
       </c>
@@ -7483,7 +7482,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>41210</v>
       </c>
@@ -7503,7 +7502,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>41220</v>
       </c>
@@ -7523,7 +7522,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>41221</v>
       </c>
@@ -7543,7 +7542,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>41300</v>
       </c>
@@ -7563,7 +7562,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>41301</v>
       </c>
@@ -7583,7 +7582,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>41302</v>
       </c>
@@ -7603,7 +7602,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>41310</v>
       </c>
@@ -7623,7 +7622,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>41311</v>
       </c>
@@ -7643,7 +7642,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>41320</v>
       </c>
@@ -7663,7 +7662,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>41321</v>
       </c>
@@ -7683,7 +7682,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>41400</v>
       </c>
@@ -7703,7 +7702,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>41401</v>
       </c>
@@ -7723,7 +7722,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>41402</v>
       </c>
@@ -7743,7 +7742,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>41403</v>
       </c>
@@ -7763,7 +7762,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>41404</v>
       </c>
@@ -7783,7 +7782,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>41405</v>
       </c>
@@ -7803,7 +7802,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>41406</v>
       </c>
@@ -7823,7 +7822,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>41407</v>
       </c>
@@ -7843,7 +7842,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>41409</v>
       </c>
@@ -7863,7 +7862,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>42100</v>
       </c>
@@ -7883,7 +7882,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>42101</v>
       </c>
@@ -7903,7 +7902,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>42102</v>
       </c>
@@ -7923,7 +7922,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>42200</v>
       </c>
@@ -7943,7 +7942,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>42201</v>
       </c>
@@ -7963,7 +7962,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>42202</v>
       </c>
@@ -7983,7 +7982,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>42203</v>
       </c>
@@ -8003,7 +8002,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>42204</v>
       </c>
@@ -8023,7 +8022,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>43100</v>
       </c>
@@ -8043,7 +8042,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>43109</v>
       </c>
@@ -8063,7 +8062,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>43200</v>
       </c>
@@ -8083,7 +8082,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>43201</v>
       </c>
@@ -8103,7 +8102,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>43202</v>
       </c>
@@ -8123,7 +8122,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>43203</v>
       </c>
@@ -8143,7 +8142,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>43204</v>
       </c>
@@ -8163,7 +8162,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>44100</v>
       </c>
@@ -8183,7 +8182,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>44101</v>
       </c>
@@ -8203,7 +8202,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>44200</v>
       </c>
@@ -8223,7 +8222,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>45100</v>
       </c>
@@ -8243,7 +8242,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>50010</v>
       </c>
@@ -8263,7 +8262,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>50011</v>
       </c>
@@ -8283,7 +8282,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>50012</v>
       </c>
@@ -8303,7 +8302,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>51100</v>
       </c>
@@ -8323,7 +8322,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>51101</v>
       </c>
@@ -8343,7 +8342,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>51102</v>
       </c>
@@ -8363,7 +8362,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>51110</v>
       </c>
@@ -8383,7 +8382,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>51111</v>
       </c>
@@ -8403,7 +8402,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>51112</v>
       </c>
@@ -8423,7 +8422,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>51113</v>
       </c>
@@ -8443,7 +8442,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>51114</v>
       </c>
@@ -8463,7 +8462,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>51120</v>
       </c>
@@ -8483,7 +8482,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>51121</v>
       </c>
@@ -8503,7 +8502,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>51122</v>
       </c>
@@ -8523,7 +8522,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>52100</v>
       </c>
@@ -8543,7 +8542,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>52110</v>
       </c>
@@ -8563,7 +8562,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>52111</v>
       </c>
@@ -8583,7 +8582,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>52112</v>
       </c>
@@ -8603,7 +8602,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>52113</v>
       </c>
@@ -8623,7 +8622,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>52114</v>
       </c>
@@ -8643,7 +8642,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>52119</v>
       </c>
@@ -8663,7 +8662,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>52120</v>
       </c>
@@ -8683,7 +8682,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>52121</v>
       </c>
@@ -8703,7 +8702,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>53100</v>
       </c>
@@ -8723,7 +8722,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>53110</v>
       </c>
@@ -8743,7 +8742,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>53111</v>
       </c>
@@ -8763,7 +8762,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>53120</v>
       </c>
@@ -8783,7 +8782,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>53121</v>
       </c>
@@ -8803,7 +8802,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>53122</v>
       </c>
@@ -8823,7 +8822,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>53123</v>
       </c>
@@ -8843,7 +8842,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>53124</v>
       </c>
@@ -8863,7 +8862,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>53125</v>
       </c>
@@ -8883,7 +8882,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>53200</v>
       </c>
@@ -8903,7 +8902,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>53201</v>
       </c>
@@ -8923,7 +8922,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>53202</v>
       </c>
@@ -8943,7 +8942,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>54100</v>
       </c>
@@ -8963,7 +8962,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>55109</v>
       </c>
@@ -8983,7 +8982,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>60010</v>
       </c>
@@ -9003,7 +9002,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>60020</v>
       </c>
@@ -9023,7 +9022,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>60030</v>
       </c>
@@ -9043,7 +9042,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>60031</v>
       </c>
@@ -9063,7 +9062,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>60040</v>
       </c>
@@ -9083,7 +9082,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>62010</v>
       </c>
@@ -9103,7 +9102,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>62020</v>
       </c>
@@ -9123,7 +9122,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>62021</v>
       </c>
@@ -9143,7 +9142,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>62022</v>
       </c>
@@ -9163,7 +9162,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>62023</v>
       </c>
@@ -9183,7 +9182,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>62024</v>
       </c>
@@ -9203,7 +9202,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>62029</v>
       </c>
@@ -9223,7 +9222,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>62100</v>
       </c>
@@ -9243,7 +9242,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>62101</v>
       </c>
@@ -9263,7 +9262,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>62200</v>
       </c>
@@ -9283,7 +9282,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>62201</v>
       </c>
@@ -9303,7 +9302,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>62202</v>
       </c>
@@ -9323,7 +9322,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>63100</v>
       </c>
@@ -9343,7 +9342,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>63101</v>
       </c>
@@ -9363,7 +9362,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>63102</v>
       </c>
@@ -9383,7 +9382,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>63200</v>
       </c>
@@ -9403,7 +9402,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>63201</v>
       </c>
@@ -9423,7 +9422,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>63202</v>
       </c>
@@ -9443,7 +9442,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>63210</v>
       </c>
@@ -9463,7 +9462,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>63211</v>
       </c>
@@ -9483,7 +9482,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>63220</v>
       </c>
@@ -9503,7 +9502,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>63221</v>
       </c>
@@ -9523,7 +9522,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>64100</v>
       </c>
@@ -9543,7 +9542,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>64101</v>
       </c>
@@ -9563,7 +9562,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>64200</v>
       </c>
@@ -9583,7 +9582,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>64201</v>
       </c>
@@ -9603,7 +9602,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>64300</v>
       </c>
@@ -9623,7 +9622,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>64301</v>
       </c>
@@ -9643,7 +9642,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>64310</v>
       </c>
@@ -9663,7 +9662,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>64311</v>
       </c>
@@ -9683,7 +9682,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>64312</v>
       </c>
@@ -9703,7 +9702,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>64313</v>
       </c>
@@ -9723,7 +9722,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>64314</v>
       </c>
@@ -9743,7 +9742,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>64320</v>
       </c>
@@ -9763,7 +9762,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>64321</v>
       </c>
@@ -9783,7 +9782,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>64322</v>
       </c>
@@ -9803,7 +9802,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>64400</v>
       </c>
@@ -9823,7 +9822,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>64401</v>
       </c>
@@ -9843,7 +9842,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>64409</v>
       </c>
@@ -9863,7 +9862,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>64410</v>
       </c>
@@ -9883,7 +9882,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>65100</v>
       </c>
@@ -9903,7 +9902,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>65101</v>
       </c>
@@ -9923,7 +9922,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>65102</v>
       </c>
@@ -9943,7 +9942,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>65109</v>
       </c>
@@ -9963,7 +9962,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>65200</v>
       </c>
@@ -9983,7 +9982,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>65201</v>
       </c>
@@ -10003,7 +10002,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>65202</v>
       </c>
@@ -10023,7 +10022,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>65210</v>
       </c>
@@ -10043,7 +10042,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>65211</v>
       </c>
@@ -10063,7 +10062,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>65220</v>
       </c>
@@ -10083,7 +10082,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>65229</v>
       </c>
@@ -10103,7 +10102,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>65310</v>
       </c>
@@ -10123,7 +10122,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>65311</v>
       </c>
@@ -10143,7 +10142,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>65312</v>
       </c>
@@ -10163,7 +10162,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>65320</v>
       </c>
@@ -10183,7 +10182,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>65329</v>
       </c>
@@ -10203,7 +10202,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>70010</v>
       </c>
@@ -10223,7 +10222,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>70011</v>
       </c>
@@ -10243,7 +10242,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>70012</v>
       </c>
@@ -10263,7 +10262,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>70020</v>
       </c>
@@ -10283,7 +10282,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>70021</v>
       </c>
@@ -10303,7 +10302,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>72010</v>
       </c>
@@ -10323,7 +10322,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>72011</v>
       </c>
@@ -10343,7 +10342,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>72012</v>
       </c>
@@ -10363,7 +10362,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>72013</v>
       </c>
@@ -10383,7 +10382,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>72014</v>
       </c>
@@ -10403,7 +10402,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>72020</v>
       </c>
@@ -10423,7 +10422,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>72021</v>
       </c>
@@ -10443,7 +10442,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>72022</v>
       </c>
@@ -10463,7 +10462,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>72023</v>
       </c>
@@ -10483,7 +10482,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>72024</v>
       </c>
@@ -10503,7 +10502,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>72025</v>
       </c>
@@ -10523,7 +10522,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>72100</v>
       </c>
@@ -10543,7 +10542,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>72101</v>
       </c>
@@ -10563,7 +10562,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>72102</v>
       </c>
@@ -10583,7 +10582,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>72103</v>
       </c>
@@ -10603,7 +10602,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>72104</v>
       </c>
@@ -10623,7 +10622,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>72105</v>
       </c>
@@ -10643,7 +10642,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>72106</v>
       </c>
@@ -10663,7 +10662,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>72200</v>
       </c>
@@ -10683,7 +10682,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>72201</v>
       </c>
@@ -10703,7 +10702,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>72202</v>
       </c>
@@ -10723,7 +10722,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>72203</v>
       </c>
@@ -10743,7 +10742,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>72204</v>
       </c>
@@ -10763,7 +10762,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>72205</v>
       </c>
@@ -10783,7 +10782,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>72300</v>
       </c>
@@ -10803,7 +10802,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>72301</v>
       </c>
@@ -10823,7 +10822,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>72302</v>
       </c>
@@ -10843,7 +10842,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>72310</v>
       </c>
@@ -10863,7 +10862,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>72311</v>
       </c>
@@ -10883,7 +10882,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>72320</v>
       </c>
@@ -10903,7 +10902,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>72321</v>
       </c>
@@ -10923,7 +10922,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>72400</v>
       </c>
@@ -10943,7 +10942,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>72401</v>
       </c>
@@ -10963,7 +10962,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>72402</v>
       </c>
@@ -10983,7 +10982,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>72403</v>
       </c>
@@ -11003,7 +11002,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>72404</v>
       </c>
@@ -11023,7 +11022,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>72405</v>
       </c>
@@ -11043,7 +11042,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>72406</v>
       </c>
@@ -11063,7 +11062,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>72410</v>
       </c>
@@ -11083,7 +11082,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>72411</v>
       </c>
@@ -11103,7 +11102,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>72420</v>
       </c>
@@ -11123,7 +11122,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>72421</v>
       </c>
@@ -11143,7 +11142,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>72422</v>
       </c>
@@ -11163,7 +11162,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>72423</v>
       </c>
@@ -11183,7 +11182,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>72429</v>
       </c>
@@ -11203,7 +11202,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>72500</v>
       </c>
@@ -11223,7 +11222,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>72501</v>
       </c>
@@ -11243,7 +11242,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>72600</v>
       </c>
@@ -11263,7 +11262,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>72601</v>
       </c>
@@ -11283,7 +11282,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>72602</v>
       </c>
@@ -11303,7 +11302,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>72603</v>
       </c>
@@ -11323,7 +11322,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>72604</v>
       </c>
@@ -11343,7 +11342,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>72999</v>
       </c>
@@ -11363,7 +11362,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>73100</v>
       </c>
@@ -11383,7 +11382,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>73101</v>
       </c>
@@ -11403,7 +11402,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>73102</v>
       </c>
@@ -11423,7 +11422,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>73110</v>
       </c>
@@ -11443,7 +11442,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>73111</v>
       </c>
@@ -11463,7 +11462,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>73112</v>
       </c>
@@ -11483,7 +11482,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>73113</v>
       </c>
@@ -11503,7 +11502,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>73200</v>
       </c>
@@ -11523,7 +11522,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>73201</v>
       </c>
@@ -11543,7 +11542,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>73202</v>
       </c>
@@ -11563,7 +11562,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>73209</v>
       </c>
@@ -11583,7 +11582,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>73300</v>
       </c>
@@ -11603,7 +11602,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>73301</v>
       </c>
@@ -11623,7 +11622,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>73310</v>
       </c>
@@ -11643,7 +11642,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>73311</v>
       </c>
@@ -11663,7 +11662,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>73400</v>
       </c>
@@ -11683,7 +11682,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>73401</v>
       </c>
@@ -11703,7 +11702,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>73402</v>
       </c>
@@ -11723,7 +11722,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>74100</v>
       </c>
@@ -11743,7 +11742,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>74101</v>
       </c>
@@ -11763,7 +11762,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>74102</v>
       </c>
@@ -11783,7 +11782,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>74200</v>
       </c>
@@ -11803,7 +11802,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>74201</v>
       </c>
@@ -11823,7 +11822,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>74202</v>
       </c>
@@ -11843,7 +11842,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>74203</v>
       </c>
@@ -11863,7 +11862,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>74204</v>
       </c>
@@ -11883,7 +11882,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>74205</v>
       </c>
@@ -11903,7 +11902,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>75100</v>
       </c>
@@ -11923,7 +11922,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>75101</v>
       </c>
@@ -11943,7 +11942,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>75110</v>
       </c>
@@ -11963,7 +11962,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>75119</v>
       </c>
@@ -11983,7 +11982,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>75200</v>
       </c>
@@ -12003,7 +12002,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>75201</v>
       </c>
@@ -12023,7 +12022,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>75210</v>
       </c>
@@ -12043,7 +12042,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="419" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>75211</v>
       </c>
@@ -12063,7 +12062,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="420" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>75212</v>
       </c>
@@ -12083,7 +12082,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>80010</v>
       </c>
@@ -12103,7 +12102,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="422" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>80020</v>
       </c>
@@ -12123,7 +12122,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>80021</v>
       </c>
@@ -12143,7 +12142,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>80022</v>
       </c>
@@ -12163,7 +12162,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>82010</v>
       </c>
@@ -12183,7 +12182,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>82020</v>
       </c>
@@ -12203,7 +12202,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>82021</v>
       </c>
@@ -12223,7 +12222,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="428" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>82030</v>
       </c>
@@ -12243,7 +12242,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="429" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>82031</v>
       </c>
@@ -12263,7 +12262,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="430" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>83100</v>
       </c>
@@ -12283,7 +12282,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="431" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>83101</v>
       </c>
@@ -12303,7 +12302,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="432" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>83110</v>
       </c>
@@ -12323,7 +12322,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>83120</v>
       </c>
@@ -12343,7 +12342,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>83121</v>
       </c>
@@ -12363,7 +12362,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="435" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>84100</v>
       </c>
@@ -12383,7 +12382,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="436" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>84101</v>
       </c>
@@ -12403,7 +12402,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="437" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>84110</v>
       </c>
@@ -12423,7 +12422,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="438" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>84111</v>
       </c>
@@ -12443,7 +12442,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="439" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>84120</v>
       </c>
@@ -12463,7 +12462,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="440" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>84121</v>
       </c>
@@ -12483,7 +12482,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>85100</v>
       </c>
@@ -12503,7 +12502,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>85101</v>
       </c>
@@ -12523,7 +12522,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>85102</v>
       </c>
@@ -12543,7 +12542,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>85103</v>
       </c>
@@ -12563,7 +12562,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>85104</v>
       </c>
@@ -12583,7 +12582,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>85110</v>
       </c>
@@ -12603,7 +12602,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>85111</v>
       </c>
@@ -12623,7 +12622,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="448" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>85120</v>
       </c>
@@ -12643,7 +12642,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="449" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>85121</v>
       </c>
@@ -12663,7 +12662,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="450" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>90010</v>
       </c>
@@ -12683,7 +12682,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="451" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>90011</v>
       </c>
@@ -12703,7 +12702,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="452" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>92010</v>
       </c>
@@ -12723,7 +12722,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>92011</v>
       </c>
@@ -12743,7 +12742,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="454" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>92012</v>
       </c>
@@ -12763,7 +12762,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A455">
         <v>92013</v>
       </c>
@@ -12783,7 +12782,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="456" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A456">
         <v>92014</v>
       </c>
@@ -12803,7 +12802,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="457" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A457">
         <v>92015</v>
       </c>
@@ -12823,7 +12822,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A458">
         <v>92020</v>
       </c>
@@ -12843,7 +12842,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="459" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>92021</v>
       </c>
@@ -12863,7 +12862,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="460" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A460">
         <v>92022</v>
       </c>
@@ -12883,7 +12882,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A461">
         <v>92023</v>
       </c>
@@ -12903,7 +12902,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A462">
         <v>92024</v>
       </c>
@@ -12923,7 +12922,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="463" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A463">
         <v>92100</v>
       </c>
@@ -12943,7 +12942,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="464" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A464">
         <v>92101</v>
       </c>
@@ -12963,7 +12962,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="465" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A465">
         <v>93100</v>
       </c>
@@ -12983,7 +12982,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="466" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A466">
         <v>93101</v>
       </c>
@@ -13003,7 +13002,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="467" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A467">
         <v>93102</v>
       </c>
@@ -13023,7 +13022,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="468" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A468">
         <v>93200</v>
       </c>
@@ -13043,7 +13042,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="469" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A469">
         <v>94100</v>
       </c>
@@ -13063,7 +13062,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="470" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A470">
         <v>94101</v>
       </c>
@@ -13083,7 +13082,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="471" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A471">
         <v>94102</v>
       </c>
@@ -13103,7 +13102,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="472" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A472">
         <v>94103</v>
       </c>
@@ -13123,7 +13122,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="473" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A473">
         <v>94104</v>
       </c>
@@ -13143,7 +13142,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="474" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A474">
         <v>94105</v>
       </c>
@@ -13163,7 +13162,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="475" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A475">
         <v>94106</v>
       </c>
@@ -13183,7 +13182,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="476" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A476">
         <v>94107</v>
       </c>
@@ -13203,7 +13202,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="477" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A477">
         <v>94110</v>
       </c>
@@ -13223,7 +13222,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="478" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A478">
         <v>94111</v>
       </c>
@@ -13243,7 +13242,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="479" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A479">
         <v>94112</v>
       </c>
@@ -13263,7 +13262,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="480" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A480">
         <v>94120</v>
       </c>
@@ -13283,7 +13282,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="481" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A481">
         <v>94121</v>
       </c>
@@ -13303,7 +13302,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="482" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A482">
         <v>94122</v>
       </c>
@@ -13323,7 +13322,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="483" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A483">
         <v>94123</v>
       </c>
@@ -13343,7 +13342,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="484" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A484">
         <v>94124</v>
       </c>
@@ -13363,7 +13362,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="485" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A485">
         <v>94129</v>
       </c>
@@ -13383,7 +13382,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="486" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A486">
         <v>94130</v>
       </c>
@@ -13403,7 +13402,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="487" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A487">
         <v>94131</v>
       </c>
@@ -13423,7 +13422,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="488" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A488">
         <v>94132</v>
       </c>
@@ -13443,7 +13442,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="489" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A489">
         <v>94133</v>
       </c>
@@ -13463,7 +13462,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="490" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A490">
         <v>94140</v>
       </c>
@@ -13483,7 +13482,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="491" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A491">
         <v>94141</v>
       </c>
@@ -13503,7 +13502,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="492" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A492">
         <v>94142</v>
       </c>
@@ -13523,7 +13522,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="493" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A493">
         <v>94143</v>
       </c>
@@ -13543,7 +13542,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="494" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A494">
         <v>94150</v>
       </c>
@@ -13563,7 +13562,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="495" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>94151</v>
       </c>
@@ -13583,7 +13582,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="496" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>94152</v>
       </c>
@@ -13603,7 +13602,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="497" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>94153</v>
       </c>
@@ -13623,7 +13622,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="498" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>94200</v>
       </c>
@@ -13643,7 +13642,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="499" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>94201</v>
       </c>
@@ -13663,7 +13662,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="500" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>94202</v>
       </c>
@@ -13683,7 +13682,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="501" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A501">
         <v>94203</v>
       </c>
@@ -13703,7 +13702,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="502" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A502">
         <v>94204</v>
       </c>
@@ -13723,7 +13722,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="503" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A503">
         <v>94205</v>
       </c>
@@ -13743,7 +13742,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="504" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A504">
         <v>94210</v>
       </c>
@@ -13763,7 +13762,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="505" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A505">
         <v>94211</v>
       </c>
@@ -13783,7 +13782,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="506" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A506">
         <v>94212</v>
       </c>
@@ -13803,7 +13802,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="507" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A507">
         <v>94213</v>
       </c>
@@ -13823,7 +13822,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="508" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A508">
         <v>94219</v>
       </c>
@@ -13843,7 +13842,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="509" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A509">
         <v>95100</v>
       </c>
@@ -13863,7 +13862,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="510" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A510">
         <v>95101</v>
       </c>
@@ -13883,7 +13882,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="511" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A511">
         <v>95102</v>
       </c>
@@ -13903,7 +13902,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="512" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A512">
         <v>95103</v>
       </c>
@@ -13923,7 +13922,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="513" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A513">
         <v>95104</v>
       </c>
@@ -13943,7 +13942,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="514" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A514">
         <v>95105</v>
       </c>
@@ -13963,7 +13962,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="515" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A515">
         <v>95106</v>
       </c>
@@ -13983,7 +13982,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="516" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A516">
         <v>95107</v>
       </c>
@@ -14003,7 +14002,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="517" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A517">
         <v>95109</v>
       </c>
@@ -14024,18 +14023,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F517" xr:uid="{C73F14DE-B5AF-457D-BD84-E38D1B6C52C5}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Léger déficit"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Business, finance and administration occupations"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F517" xr:uid="{C73F14DE-B5AF-457D-BD84-E38D1B6C52C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>